<commit_message>
added logistic regression scores
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Final Results" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
   <si>
     <t>Classifier</t>
   </si>
@@ -62,12 +62,18 @@
   <si>
     <t>k-Nearest Neighbour Classification</t>
   </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,6 +106,22 @@
     <font>
       <sz val="18"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,18 +159,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -575,10 +602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X44"/>
+  <dimension ref="B1:X87"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="126" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3072,7 +3099,848 @@
         <v>0.78920000000000001</v>
       </c>
     </row>
+    <row r="46" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3</v>
+      </c>
+      <c r="G48" s="1">
+        <v>4</v>
+      </c>
+      <c r="H48" s="1">
+        <v>5</v>
+      </c>
+      <c r="I48" s="1">
+        <v>6</v>
+      </c>
+      <c r="J48" s="1">
+        <v>7</v>
+      </c>
+      <c r="K48" s="1">
+        <v>8</v>
+      </c>
+      <c r="L48" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B49" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.90874999999999995</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0.93374999999999997</v>
+      </c>
+      <c r="K49" s="2">
+        <v>0.90375000000000005</v>
+      </c>
+      <c r="L49" s="2">
+        <v>0.91874999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B50" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.91625000000000001</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.89249999999999996</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0.91625000000000001</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="K50" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L50" s="2">
+        <v>0.92249999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B51" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.91625000000000001</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.89124999999999999</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0.91749999999999998</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0.92125000000000001</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="J51" s="2">
+        <v>0.93374999999999997</v>
+      </c>
+      <c r="K51" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="L51" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B52" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.89124999999999999</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.91625000000000001</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.92125000000000001</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.89875000000000005</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0.93374999999999997</v>
+      </c>
+      <c r="K52" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="L52" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B53" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.92125000000000001</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0.89375000000000004</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0.93374999999999997</v>
+      </c>
+      <c r="K53" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="L53" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B54" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.90375000000000005</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0.89375000000000004</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="G54" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+      <c r="I54" s="2">
+        <v>0.89624999999999999</v>
+      </c>
+      <c r="J54" s="2">
+        <v>0.9325</v>
+      </c>
+      <c r="K54" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="L54" s="2">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B55" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0.89375000000000004</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+      <c r="I55" s="2">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="J55" s="2">
+        <v>0.9325</v>
+      </c>
+      <c r="K55" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="L55" s="2">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B56" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0.89375000000000004</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="J56" s="2">
+        <v>0.93125000000000002</v>
+      </c>
+      <c r="K56" s="2">
+        <v>0.90125</v>
+      </c>
+      <c r="L56" s="2">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B57" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0.89375000000000004</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0.91874999999999996</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="J57" s="2">
+        <v>0.93125000000000002</v>
+      </c>
+      <c r="K57" s="2">
+        <v>0.90125</v>
+      </c>
+      <c r="L57" s="2">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B58" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0.89249999999999996</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0.91874999999999996</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="J58" s="2">
+        <v>0.93125000000000002</v>
+      </c>
+      <c r="K58" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L58" s="2">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B59" s="6">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0.89124999999999999</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="G59" s="2">
+        <v>0.91874999999999996</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0.92374999999999996</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="J59" s="2">
+        <v>0.9325</v>
+      </c>
+      <c r="K59" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="L59" s="2">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
+        <v>2</v>
+      </c>
+      <c r="F62" s="1">
+        <v>3</v>
+      </c>
+      <c r="G62" s="1">
+        <v>4</v>
+      </c>
+      <c r="H62" s="1">
+        <v>5</v>
+      </c>
+      <c r="I62" s="1">
+        <v>6</v>
+      </c>
+      <c r="J62" s="1">
+        <v>7</v>
+      </c>
+      <c r="K62" s="1">
+        <v>8</v>
+      </c>
+      <c r="L62" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B63" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B64" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B65" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B66" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B67" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B68" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B69" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B70" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B71" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B72" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B73" s="6">
+        <v>1</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="1">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2</v>
+      </c>
+      <c r="F76" s="1">
+        <v>3</v>
+      </c>
+      <c r="G76" s="1">
+        <v>4</v>
+      </c>
+      <c r="H76" s="1">
+        <v>5</v>
+      </c>
+      <c r="I76" s="1">
+        <v>6</v>
+      </c>
+      <c r="J76" s="1">
+        <v>7</v>
+      </c>
+      <c r="K76" s="1">
+        <v>8</v>
+      </c>
+      <c r="L76" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B77" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B78" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B79" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B80" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B81" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B82" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B83" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B84" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B85" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B86" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B87" s="6">
+        <v>1</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="2"/>
+      <c r="K87" s="2"/>
+      <c r="L87" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added sections needed for the report
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -732,7 +732,7 @@
   <dimension ref="B1:X155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J133" zoomScale="114" workbookViewId="0">
-      <selection activeCell="N151" sqref="N151:N155"/>
+      <selection activeCell="T155" sqref="T155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8304,16 +8304,36 @@
       <c r="N135" s="9">
         <v>10</v>
       </c>
-      <c r="O135" s="2"/>
-      <c r="P135" s="2"/>
-      <c r="Q135" s="2"/>
-      <c r="R135" s="2"/>
-      <c r="S135" s="2"/>
-      <c r="T135" s="2"/>
-      <c r="U135" s="2"/>
-      <c r="V135" s="2"/>
-      <c r="W135" s="2"/>
-      <c r="X135" s="2"/>
+      <c r="O135" s="2">
+        <v>0.87375000000000003</v>
+      </c>
+      <c r="P135" s="2">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="Q135" s="2">
+        <v>0.84875</v>
+      </c>
+      <c r="R135" s="2">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="S135" s="2">
+        <v>0.86624999999999996</v>
+      </c>
+      <c r="T135" s="2">
+        <v>0.86875000000000002</v>
+      </c>
+      <c r="U135" s="2">
+        <v>0.86750000000000005</v>
+      </c>
+      <c r="V135" s="2">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="W135" s="2">
+        <v>0.84750000000000003</v>
+      </c>
+      <c r="X135" s="2">
+        <v>0.87124999999999997</v>
+      </c>
     </row>
     <row r="136" spans="2:24" ht="24" x14ac:dyDescent="0.3">
       <c r="B136" s="4">
@@ -8352,14 +8372,36 @@
       <c r="N136" s="9">
         <v>50</v>
       </c>
-      <c r="O136" s="2"/>
-      <c r="R136" s="2"/>
-      <c r="S136" s="2"/>
-      <c r="T136" s="2"/>
-      <c r="U136" s="2"/>
-      <c r="V136" s="2"/>
-      <c r="W136" s="2"/>
-      <c r="X136" s="5"/>
+      <c r="O136" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="P136">
+        <v>0.88624999999999998</v>
+      </c>
+      <c r="Q136">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="R136" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="S136" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="T136" s="2">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="U136" s="2">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="V136" s="2">
+        <v>0.89875000000000005</v>
+      </c>
+      <c r="W136" s="2">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="X136" s="3">
+        <v>0.88124999999999998</v>
+      </c>
     </row>
     <row r="137" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B137" s="1">
@@ -8398,16 +8440,36 @@
       <c r="N137" s="9">
         <v>100</v>
       </c>
-      <c r="O137" s="2"/>
-      <c r="P137" s="2"/>
-      <c r="Q137" s="2"/>
-      <c r="R137" s="2"/>
-      <c r="S137" s="2"/>
-      <c r="T137" s="2"/>
-      <c r="U137" s="2"/>
-      <c r="V137" s="2"/>
-      <c r="W137" s="2"/>
-      <c r="X137" s="2"/>
+      <c r="O137" s="2">
+        <v>0.87875000000000003</v>
+      </c>
+      <c r="P137" s="2">
+        <v>0.88624999999999998</v>
+      </c>
+      <c r="Q137" s="2">
+        <v>0.86624999999999996</v>
+      </c>
+      <c r="R137" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="S137" s="2">
+        <v>0.88624999999999998</v>
+      </c>
+      <c r="T137" s="2">
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="U137" s="2">
+        <v>0.87624999999999997</v>
+      </c>
+      <c r="V137" s="2">
+        <v>0.89875000000000005</v>
+      </c>
+      <c r="W137" s="2">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="X137" s="2">
+        <v>0.88749999999999996</v>
+      </c>
     </row>
     <row r="138" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B138" s="1">
@@ -8446,16 +8508,36 @@
       <c r="N138" s="9">
         <v>150</v>
       </c>
-      <c r="O138" s="2"/>
-      <c r="P138" s="2"/>
-      <c r="Q138" s="2"/>
-      <c r="R138" s="2"/>
-      <c r="S138" s="2"/>
-      <c r="T138" s="2"/>
-      <c r="U138" s="2"/>
-      <c r="V138" s="2"/>
-      <c r="W138" s="2"/>
-      <c r="X138" s="2"/>
+      <c r="O138" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="P138" s="2">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="Q138" s="2">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="R138" s="2">
+        <v>0.88624999999999998</v>
+      </c>
+      <c r="S138" s="2">
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="T138" s="2">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="U138" s="2">
+        <v>0.87875000000000003</v>
+      </c>
+      <c r="V138" s="2">
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="W138" s="2">
+        <v>0.86875000000000002</v>
+      </c>
+      <c r="X138" s="2">
+        <v>0.88624999999999998</v>
+      </c>
     </row>
     <row r="139" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B139" s="6">
@@ -8494,16 +8576,36 @@
       <c r="N139" s="8">
         <v>200</v>
       </c>
-      <c r="O139" s="2"/>
-      <c r="P139" s="2"/>
-      <c r="Q139" s="2"/>
-      <c r="R139" s="2"/>
-      <c r="S139" s="2"/>
-      <c r="T139" s="2"/>
-      <c r="U139" s="2"/>
-      <c r="V139" s="2"/>
-      <c r="W139" s="2"/>
-      <c r="X139" s="2"/>
+      <c r="O139" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="P139" s="2">
+        <v>0.88375000000000004</v>
+      </c>
+      <c r="Q139" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="R139" s="2">
+        <v>0.88749999999999996</v>
+      </c>
+      <c r="S139" s="2">
+        <v>0.88624999999999998</v>
+      </c>
+      <c r="T139" s="2">
+        <v>0.88249999999999995</v>
+      </c>
+      <c r="U139" s="2">
+        <v>0.87875000000000003</v>
+      </c>
+      <c r="V139" s="2">
+        <v>0.89875000000000005</v>
+      </c>
+      <c r="W139" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="X139" s="2">
+        <v>0.88375000000000004</v>
+      </c>
     </row>
     <row r="141" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
@@ -8618,16 +8720,36 @@
       <c r="N143" s="9">
         <v>10</v>
       </c>
-      <c r="O143" s="2"/>
-      <c r="P143" s="2"/>
-      <c r="Q143" s="2"/>
-      <c r="R143" s="2"/>
-      <c r="S143" s="2"/>
-      <c r="T143" s="2"/>
-      <c r="U143" s="2"/>
-      <c r="V143" s="2"/>
-      <c r="W143" s="2"/>
-      <c r="X143" s="2"/>
+      <c r="O143" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="P143" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="Q143" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="R143" s="2">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="S143" s="2">
+        <v>0.78125</v>
+      </c>
+      <c r="T143" s="2">
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="U143" s="2">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="V143" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="W143" s="2">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="X143" s="2">
+        <v>0.73124999999999996</v>
+      </c>
     </row>
     <row r="144" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B144" s="1">
@@ -8666,16 +8788,36 @@
       <c r="N144" s="9">
         <v>50</v>
       </c>
-      <c r="O144" s="2"/>
-      <c r="P144" s="2"/>
-      <c r="Q144" s="2"/>
-      <c r="R144" s="2"/>
-      <c r="S144" s="2"/>
-      <c r="T144" s="2"/>
-      <c r="U144" s="2"/>
-      <c r="V144" s="2"/>
-      <c r="W144" s="2"/>
-      <c r="X144" s="2"/>
+      <c r="O144" s="2">
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="P144" s="2">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="Q144" s="2">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="R144" s="2">
+        <v>0.78125</v>
+      </c>
+      <c r="S144" s="2">
+        <v>0.79374999999999996</v>
+      </c>
+      <c r="T144" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="U144" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="V144" s="2">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="W144" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="X144" s="2">
+        <v>0.78749999999999998</v>
+      </c>
     </row>
     <row r="145" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B145" s="1">
@@ -8714,16 +8856,36 @@
       <c r="N145" s="9">
         <v>100</v>
       </c>
-      <c r="O145" s="2"/>
-      <c r="P145" s="2"/>
-      <c r="Q145" s="2"/>
-      <c r="R145" s="2"/>
-      <c r="S145" s="2"/>
-      <c r="T145" s="2"/>
-      <c r="U145" s="2"/>
-      <c r="V145" s="2"/>
-      <c r="W145" s="2"/>
-      <c r="X145" s="2"/>
+      <c r="O145" s="2">
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="P145" s="2">
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="Q145" s="2">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="R145" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="S145" s="2">
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="T145" s="2">
+        <v>0.79374999999999996</v>
+      </c>
+      <c r="U145" s="2">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="V145" s="2">
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="W145" s="2">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="X145" s="2">
+        <v>0.83125000000000004</v>
+      </c>
     </row>
     <row r="146" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B146" s="1">
@@ -8762,16 +8924,36 @@
       <c r="N146" s="9">
         <v>150</v>
       </c>
-      <c r="O146" s="2"/>
-      <c r="P146" s="2"/>
-      <c r="Q146" s="2"/>
-      <c r="R146" s="2"/>
-      <c r="S146" s="2"/>
-      <c r="T146" s="2"/>
-      <c r="U146" s="2"/>
-      <c r="V146" s="2"/>
-      <c r="W146" s="2"/>
-      <c r="X146" s="2"/>
+      <c r="O146" s="2">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="P146" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="Q146" s="2">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="R146" s="2">
+        <v>0.78125</v>
+      </c>
+      <c r="S146" s="2">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="T146" s="2">
+        <v>0.79374999999999996</v>
+      </c>
+      <c r="U146" s="2">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="V146" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="W146" s="2">
+        <v>0.84375</v>
+      </c>
+      <c r="X146" s="2">
+        <v>0.83750000000000002</v>
+      </c>
     </row>
     <row r="147" spans="2:24" ht="24" x14ac:dyDescent="0.3">
       <c r="B147" s="7">
@@ -8810,16 +8992,36 @@
       <c r="N147" s="8">
         <v>200</v>
       </c>
-      <c r="O147" s="2"/>
-      <c r="P147" s="2"/>
-      <c r="Q147" s="2"/>
-      <c r="R147" s="2"/>
-      <c r="S147" s="2"/>
-      <c r="T147" s="2"/>
-      <c r="U147" s="2"/>
-      <c r="V147" s="2"/>
-      <c r="W147" s="2"/>
-      <c r="X147" s="5"/>
+      <c r="O147" s="2">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="P147" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="Q147" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="R147" s="2">
+        <v>0.79374999999999996</v>
+      </c>
+      <c r="S147" s="2">
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="T147" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="U147" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="V147" s="2">
+        <v>0.78125</v>
+      </c>
+      <c r="W147" s="2">
+        <v>0.83750000000000002</v>
+      </c>
+      <c r="X147" s="3">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="149" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
@@ -8934,16 +9136,36 @@
       <c r="N151" s="9">
         <v>10</v>
       </c>
-      <c r="O151" s="2"/>
-      <c r="P151" s="2"/>
-      <c r="Q151" s="2"/>
-      <c r="R151" s="2"/>
-      <c r="S151" s="2"/>
-      <c r="T151" s="2"/>
-      <c r="U151" s="2"/>
-      <c r="V151" s="2"/>
-      <c r="W151" s="2"/>
-      <c r="X151" s="2"/>
+      <c r="O151" s="2">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="P151" s="2">
+        <v>0.78879999999999995</v>
+      </c>
+      <c r="Q151" s="2">
+        <v>0.78520000000000001</v>
+      </c>
+      <c r="R151" s="2">
+        <v>0.80879999999999996</v>
+      </c>
+      <c r="S151" s="2">
+        <v>0.80559999999999998</v>
+      </c>
+      <c r="T151" s="2">
+        <v>0.79320000000000002</v>
+      </c>
+      <c r="U151" s="2">
+        <v>0.78039999999999998</v>
+      </c>
+      <c r="V151" s="2">
+        <v>0.78839999999999999</v>
+      </c>
+      <c r="W151" s="2">
+        <v>0.82320000000000004</v>
+      </c>
+      <c r="X151" s="2">
+        <v>0.7944</v>
+      </c>
     </row>
     <row r="152" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B152" s="1">
@@ -8982,16 +9204,36 @@
       <c r="N152" s="9">
         <v>50</v>
       </c>
-      <c r="O152" s="2"/>
-      <c r="P152" s="2"/>
-      <c r="Q152" s="2"/>
-      <c r="R152" s="2"/>
-      <c r="S152" s="2"/>
-      <c r="T152" s="2"/>
-      <c r="U152" s="2"/>
-      <c r="V152" s="2"/>
-      <c r="W152" s="2"/>
-      <c r="X152" s="2"/>
+      <c r="O152" s="2">
+        <v>0.83960000000000001</v>
+      </c>
+      <c r="P152">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="Q152" s="2">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="R152" s="2">
+        <v>0.83079999999999998</v>
+      </c>
+      <c r="S152" s="2">
+        <v>0.82720000000000005</v>
+      </c>
+      <c r="T152" s="2">
+        <v>0.82679999999999998</v>
+      </c>
+      <c r="U152" s="2">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="V152" s="2">
+        <v>0.83840000000000003</v>
+      </c>
+      <c r="W152" s="2">
+        <v>0.83160000000000001</v>
+      </c>
+      <c r="X152" s="2">
+        <v>0.81799999999999995</v>
+      </c>
     </row>
     <row r="153" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B153" s="1">
@@ -9030,16 +9272,36 @@
       <c r="N153" s="9">
         <v>100</v>
       </c>
-      <c r="O153" s="2"/>
-      <c r="P153" s="2"/>
-      <c r="Q153" s="2"/>
-      <c r="R153" s="2"/>
-      <c r="S153" s="2"/>
-      <c r="T153" s="2"/>
-      <c r="U153" s="2"/>
-      <c r="V153" s="2"/>
-      <c r="W153" s="2"/>
-      <c r="X153" s="2"/>
+      <c r="O153" s="2">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="P153" s="2">
+        <v>0.82640000000000002</v>
+      </c>
+      <c r="Q153" s="2">
+        <v>0.80879999999999996</v>
+      </c>
+      <c r="R153" s="2">
+        <v>0.83160000000000001</v>
+      </c>
+      <c r="S153" s="2">
+        <v>0.83679999999999999</v>
+      </c>
+      <c r="T153" s="2">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="U153" s="2">
+        <v>0.81759999999999999</v>
+      </c>
+      <c r="V153" s="2">
+        <v>0.82640000000000002</v>
+      </c>
+      <c r="W153" s="2">
+        <v>0.84840000000000004</v>
+      </c>
+      <c r="X153" s="2">
+        <v>0.82520000000000004</v>
+      </c>
     </row>
     <row r="154" spans="2:24" ht="24" x14ac:dyDescent="0.3">
       <c r="B154" s="4">

</xml_diff>

<commit_message>
added results of Decision Trees and Random Forest
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="21">
   <si>
     <t>Classifier</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>Random Forests</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>n_estimators</t>
+  </si>
+  <si>
+    <t>max_depth</t>
   </si>
 </sst>
 </file>
@@ -189,7 +198,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -200,6 +209,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -488,7 +498,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,9 +701,15 @@
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="D10" s="2">
+        <v>0.85164835164835095</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.65749999999999997</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.71679999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -705,9 +721,15 @@
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="D11" s="2">
+        <v>0.82517482517482499</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.72648000000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -719,9 +741,15 @@
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="D12" s="2">
+        <v>0.89710289710289703</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.78847999999999996</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -733,9 +761,15 @@
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="D13" s="2">
+        <v>0.863136863136863</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.72250000000000003</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.79967999999999995</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -745,10 +779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X155"/>
+  <dimension ref="B1:X205"/>
   <sheetViews>
-    <sheetView topLeftCell="I133" zoomScale="114" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView topLeftCell="K185" zoomScale="115" workbookViewId="0">
+      <selection activeCell="O206" sqref="O206:X206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8217,7 +8251,7 @@
     </row>
     <row r="134" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B134" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C134" s="1">
         <v>0</v>
@@ -8250,7 +8284,7 @@
         <v>9</v>
       </c>
       <c r="N134" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="O134" s="1">
         <v>0</v>
@@ -8633,7 +8667,7 @@
     </row>
     <row r="142" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B142" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C142" s="1">
         <v>0</v>
@@ -8666,7 +8700,7 @@
         <v>9</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="O142" s="1">
         <v>0</v>
@@ -9049,7 +9083,7 @@
     </row>
     <row r="150" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B150" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C150" s="1">
         <v>0</v>
@@ -9082,7 +9116,7 @@
         <v>9</v>
       </c>
       <c r="N150" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="O150" s="1">
         <v>0</v>
@@ -9453,6 +9487,2518 @@
       </c>
       <c r="X155" s="2">
         <v>0.82479999999999998</v>
+      </c>
+    </row>
+    <row r="157" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B157" t="s">
+        <v>16</v>
+      </c>
+      <c r="N157" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B158" t="s">
+        <v>1</v>
+      </c>
+      <c r="N158" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B159" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C159" s="1">
+        <v>0</v>
+      </c>
+      <c r="D159" s="1">
+        <v>1</v>
+      </c>
+      <c r="E159" s="1">
+        <v>2</v>
+      </c>
+      <c r="F159" s="1">
+        <v>3</v>
+      </c>
+      <c r="G159" s="1">
+        <v>4</v>
+      </c>
+      <c r="H159" s="1">
+        <v>5</v>
+      </c>
+      <c r="I159" s="1">
+        <v>6</v>
+      </c>
+      <c r="J159" s="1">
+        <v>7</v>
+      </c>
+      <c r="K159" s="1">
+        <v>8</v>
+      </c>
+      <c r="L159" s="1">
+        <v>9</v>
+      </c>
+      <c r="N159" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O159" s="1">
+        <v>0</v>
+      </c>
+      <c r="P159" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q159" s="1">
+        <v>2</v>
+      </c>
+      <c r="R159" s="1">
+        <v>3</v>
+      </c>
+      <c r="S159" s="1">
+        <v>4</v>
+      </c>
+      <c r="T159" s="1">
+        <v>5</v>
+      </c>
+      <c r="U159" s="1">
+        <v>6</v>
+      </c>
+      <c r="V159" s="1">
+        <v>7</v>
+      </c>
+      <c r="W159" s="1">
+        <v>8</v>
+      </c>
+      <c r="X159" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="160" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B160" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C160" s="3">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="D160" s="3">
+        <v>0.85624999999999996</v>
+      </c>
+      <c r="E160" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="F160" s="3">
+        <v>0.87875000000000003</v>
+      </c>
+      <c r="G160" s="3">
+        <v>0.84875</v>
+      </c>
+      <c r="H160" s="3">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="I160" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="J160" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="K160" s="3">
+        <v>0.84875</v>
+      </c>
+      <c r="L160" s="5">
+        <v>0.89624999999999999</v>
+      </c>
+      <c r="N160" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O160" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="P160" s="2">
+        <v>0.82250000000000001</v>
+      </c>
+      <c r="Q160" s="2">
+        <v>0.82125000000000004</v>
+      </c>
+      <c r="R160" s="2">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="S160" s="2">
+        <v>0.82625000000000004</v>
+      </c>
+      <c r="T160" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="U160" s="2">
+        <v>0.82625000000000004</v>
+      </c>
+      <c r="V160" s="2">
+        <v>0.85250000000000004</v>
+      </c>
+      <c r="W160" s="2">
+        <v>0.82874999999999999</v>
+      </c>
+      <c r="X160" s="2">
+        <v>0.83125000000000004</v>
+      </c>
+    </row>
+    <row r="161" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B161" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C161" s="3">
+        <v>0.85875000000000001</v>
+      </c>
+      <c r="D161" s="10">
+        <v>0.86124999999999996</v>
+      </c>
+      <c r="E161" s="10">
+        <v>0.84</v>
+      </c>
+      <c r="F161" s="3">
+        <v>0.86875000000000002</v>
+      </c>
+      <c r="G161" s="3">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="H161" s="3">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="I161" s="3">
+        <v>0.85250000000000004</v>
+      </c>
+      <c r="J161" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="K161" s="3">
+        <v>0.85124999999999995</v>
+      </c>
+      <c r="L161" s="3">
+        <v>0.89124999999999999</v>
+      </c>
+      <c r="N161" s="9">
+        <v>1000</v>
+      </c>
+      <c r="O161" s="2">
+        <v>0.83125000000000004</v>
+      </c>
+      <c r="P161">
+        <v>0.82374999999999998</v>
+      </c>
+      <c r="Q161">
+        <v>0.8175</v>
+      </c>
+      <c r="R161" s="2">
+        <v>0.84250000000000003</v>
+      </c>
+      <c r="S161" s="2">
+        <v>0.83250000000000002</v>
+      </c>
+      <c r="T161" s="2">
+        <v>0.81874999999999998</v>
+      </c>
+      <c r="U161" s="2">
+        <v>0.81625000000000003</v>
+      </c>
+      <c r="V161" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="W161" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="X161" s="3">
+        <v>0.83750000000000002</v>
+      </c>
+    </row>
+    <row r="162" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B162" s="9">
+        <v>2000</v>
+      </c>
+      <c r="C162" s="3">
+        <v>0.85875000000000001</v>
+      </c>
+      <c r="D162" s="3">
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="E162" s="3">
+        <v>0.85250000000000004</v>
+      </c>
+      <c r="F162" s="3">
+        <v>0.87124999999999997</v>
+      </c>
+      <c r="G162" s="3">
+        <v>0.85250000000000004</v>
+      </c>
+      <c r="H162" s="3">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="I162" s="3">
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="J162" s="3">
+        <v>0.86624999999999996</v>
+      </c>
+      <c r="K162" s="3">
+        <v>0.85250000000000004</v>
+      </c>
+      <c r="L162" s="3">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="N162" s="1">
+        <v>2000</v>
+      </c>
+      <c r="O162" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="P162" s="2">
+        <v>0.82250000000000001</v>
+      </c>
+      <c r="Q162" s="2">
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="R162" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="S162" s="2">
+        <v>0.8175</v>
+      </c>
+      <c r="T162" s="2">
+        <v>0.8175</v>
+      </c>
+      <c r="U162" s="2">
+        <v>0.81125000000000003</v>
+      </c>
+      <c r="V162" s="2">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="W162" s="2">
+        <v>0.82374999999999998</v>
+      </c>
+      <c r="X162" s="2">
+        <v>0.83250000000000002</v>
+      </c>
+    </row>
+    <row r="163" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B163" s="9">
+        <v>3000</v>
+      </c>
+      <c r="C163" s="3">
+        <v>0.85624999999999996</v>
+      </c>
+      <c r="D163" s="3">
+        <v>0.85375000000000001</v>
+      </c>
+      <c r="E163" s="3">
+        <v>0.84375</v>
+      </c>
+      <c r="F163" s="3">
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="G163" s="3">
+        <v>0.84375</v>
+      </c>
+      <c r="H163" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="I163" s="3">
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="J163" s="3">
+        <v>0.86875000000000002</v>
+      </c>
+      <c r="K163" s="3">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="L163" s="3">
+        <v>0.88375000000000004</v>
+      </c>
+      <c r="N163" s="4">
+        <v>3000</v>
+      </c>
+      <c r="O163" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="P163" s="2">
+        <v>0.84250000000000003</v>
+      </c>
+      <c r="Q163" s="2">
+        <v>0.8175</v>
+      </c>
+      <c r="R163" s="5">
+        <v>0.84624999999999995</v>
+      </c>
+      <c r="S163" s="2">
+        <v>0.82750000000000001</v>
+      </c>
+      <c r="T163" s="2">
+        <v>0.80874999999999997</v>
+      </c>
+      <c r="U163" s="2">
+        <v>0.80874999999999997</v>
+      </c>
+      <c r="V163" s="2">
+        <v>0.84375</v>
+      </c>
+      <c r="W163" s="2">
+        <v>0.82250000000000001</v>
+      </c>
+      <c r="X163" s="2">
+        <v>0.83625000000000005</v>
+      </c>
+    </row>
+    <row r="164" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B164" s="8">
+        <v>4000</v>
+      </c>
+      <c r="C164" s="3">
+        <v>0.86375000000000002</v>
+      </c>
+      <c r="D164" s="3">
+        <v>0.86124999999999996</v>
+      </c>
+      <c r="E164" s="3">
+        <v>0.84624999999999995</v>
+      </c>
+      <c r="F164" s="3">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="G164" s="3">
+        <v>0.84375</v>
+      </c>
+      <c r="H164" s="3">
+        <v>0.87624999999999997</v>
+      </c>
+      <c r="I164" s="3">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J164" s="3">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="K164" s="3">
+        <v>0.84875</v>
+      </c>
+      <c r="L164" s="3">
+        <v>0.89124999999999999</v>
+      </c>
+      <c r="N164" s="6">
+        <v>4000</v>
+      </c>
+      <c r="O164" s="2">
+        <v>0.82874999999999999</v>
+      </c>
+      <c r="P164" s="2">
+        <v>0.82250000000000001</v>
+      </c>
+      <c r="Q164" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="R164" s="2">
+        <v>0.83374999999999999</v>
+      </c>
+      <c r="S164" s="2">
+        <v>0.82250000000000001</v>
+      </c>
+      <c r="T164" s="2">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="U164" s="2">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="V164" s="2">
+        <v>0.84875</v>
+      </c>
+      <c r="W164" s="2">
+        <v>0.82250000000000001</v>
+      </c>
+      <c r="X164" s="2">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="166" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B166" t="s">
+        <v>2</v>
+      </c>
+      <c r="N166" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B167" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C167" s="1">
+        <v>0</v>
+      </c>
+      <c r="D167" s="1">
+        <v>1</v>
+      </c>
+      <c r="E167" s="1">
+        <v>2</v>
+      </c>
+      <c r="F167" s="1">
+        <v>3</v>
+      </c>
+      <c r="G167" s="1">
+        <v>4</v>
+      </c>
+      <c r="H167" s="1">
+        <v>5</v>
+      </c>
+      <c r="I167" s="1">
+        <v>6</v>
+      </c>
+      <c r="J167" s="1">
+        <v>7</v>
+      </c>
+      <c r="K167" s="1">
+        <v>8</v>
+      </c>
+      <c r="L167" s="1">
+        <v>9</v>
+      </c>
+      <c r="N167" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O167" s="1">
+        <v>0</v>
+      </c>
+      <c r="P167" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q167" s="1">
+        <v>2</v>
+      </c>
+      <c r="R167" s="1">
+        <v>3</v>
+      </c>
+      <c r="S167" s="1">
+        <v>4</v>
+      </c>
+      <c r="T167" s="1">
+        <v>5</v>
+      </c>
+      <c r="U167" s="1">
+        <v>6</v>
+      </c>
+      <c r="V167" s="1">
+        <v>7</v>
+      </c>
+      <c r="W167" s="1">
+        <v>8</v>
+      </c>
+      <c r="X167" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B168" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C168" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D168" s="3">
+        <v>0.63124999999999998</v>
+      </c>
+      <c r="E168" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="F168" s="3">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="G168" s="3">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="H168" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="I168" s="3">
+        <v>0.64375000000000004</v>
+      </c>
+      <c r="J168" s="3">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="K168" s="3">
+        <v>0.64375000000000004</v>
+      </c>
+      <c r="L168" s="3">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="N168" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O168" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="P168" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="Q168" s="2">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="R168" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="S168" s="2">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="T168" s="2">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="U168" s="2">
+        <v>0.60624999999999996</v>
+      </c>
+      <c r="V168" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="W168" s="2">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="X168" s="2">
+        <v>0.66874999999999996</v>
+      </c>
+    </row>
+    <row r="169" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B169" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C169" s="3">
+        <v>0.65625</v>
+      </c>
+      <c r="D169" s="3">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="E169" s="3">
+        <v>0.61875000000000002</v>
+      </c>
+      <c r="F169" s="3">
+        <v>0.66874999999999996</v>
+      </c>
+      <c r="G169" s="3">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="H169" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="I169" s="3">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="J169" s="3">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="K169" s="3">
+        <v>0.65625</v>
+      </c>
+      <c r="L169" s="3">
+        <v>0.66874999999999996</v>
+      </c>
+      <c r="N169" s="9">
+        <v>1000</v>
+      </c>
+      <c r="O169" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="P169" s="2">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="Q169" s="2">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="R169" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="S169" s="2">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="T169" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="U169" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="V169" s="2">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="W169" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="X169" s="2">
+        <v>0.68125000000000002</v>
+      </c>
+    </row>
+    <row r="170" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B170" s="4">
+        <v>2000</v>
+      </c>
+      <c r="C170" s="3">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="D170" s="3">
+        <v>0.66874999999999996</v>
+      </c>
+      <c r="E170" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="F170" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="G170" s="3">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="H170" s="5">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="I170" s="3">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="J170" s="3">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="K170" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="L170" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="N170" s="1">
+        <v>2000</v>
+      </c>
+      <c r="O170" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="P170" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="Q170" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="R170" s="2">
+        <v>0.66874999999999996</v>
+      </c>
+      <c r="S170" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="T170" s="2">
+        <v>0.66874999999999996</v>
+      </c>
+      <c r="U170" s="2">
+        <v>0.60624999999999996</v>
+      </c>
+      <c r="V170" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="W170" s="2">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="X170" s="2">
+        <v>0.66249999999999998</v>
+      </c>
+    </row>
+    <row r="171" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B171" s="9">
+        <v>3000</v>
+      </c>
+      <c r="C171" s="3">
+        <v>0.60624999999999996</v>
+      </c>
+      <c r="D171" s="3">
+        <v>0.64375000000000004</v>
+      </c>
+      <c r="E171" s="3">
+        <v>0.64375000000000004</v>
+      </c>
+      <c r="F171" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="G171" s="3">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="H171" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="I171" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="J171" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="K171" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="L171" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="N171" s="4">
+        <v>3000</v>
+      </c>
+      <c r="O171" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="P171" s="5">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="Q171" s="2">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="R171" s="2">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="S171" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="T171" s="2">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="U171" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="V171" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="W171" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="X171" s="2">
+        <v>0.66249999999999998</v>
+      </c>
+    </row>
+    <row r="172" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B172" s="8">
+        <v>4000</v>
+      </c>
+      <c r="C172" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D172" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="E172" s="3">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="F172" s="3">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="G172" s="3">
+        <v>0.65625</v>
+      </c>
+      <c r="H172" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="I172" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="J172" s="3">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="K172" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="L172" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="N172" s="6">
+        <v>4000</v>
+      </c>
+      <c r="O172" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="P172" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="Q172" s="2">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="R172" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="S172" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="T172" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="U172" s="2">
+        <v>0.60624999999999996</v>
+      </c>
+      <c r="V172" s="2">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="W172" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="X172" s="3">
+        <v>0.64375000000000004</v>
+      </c>
+    </row>
+    <row r="174" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B174" t="s">
+        <v>3</v>
+      </c>
+      <c r="N174" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B175" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C175" s="1">
+        <v>0</v>
+      </c>
+      <c r="D175" s="1">
+        <v>1</v>
+      </c>
+      <c r="E175" s="1">
+        <v>2</v>
+      </c>
+      <c r="F175" s="1">
+        <v>3</v>
+      </c>
+      <c r="G175" s="1">
+        <v>4</v>
+      </c>
+      <c r="H175" s="1">
+        <v>5</v>
+      </c>
+      <c r="I175" s="1">
+        <v>6</v>
+      </c>
+      <c r="J175" s="1">
+        <v>7</v>
+      </c>
+      <c r="K175" s="1">
+        <v>8</v>
+      </c>
+      <c r="L175" s="1">
+        <v>9</v>
+      </c>
+      <c r="N175" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O175" s="1">
+        <v>0</v>
+      </c>
+      <c r="P175" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q175" s="1">
+        <v>2</v>
+      </c>
+      <c r="R175" s="1">
+        <v>3</v>
+      </c>
+      <c r="S175" s="1">
+        <v>4</v>
+      </c>
+      <c r="T175" s="1">
+        <v>5</v>
+      </c>
+      <c r="U175" s="1">
+        <v>6</v>
+      </c>
+      <c r="V175" s="1">
+        <v>7</v>
+      </c>
+      <c r="W175" s="1">
+        <v>8</v>
+      </c>
+      <c r="X175" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="176" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B176" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C176" s="3">
+        <v>0.71560000000000001</v>
+      </c>
+      <c r="D176" s="3">
+        <v>0.6976</v>
+      </c>
+      <c r="E176" s="3">
+        <v>0.70760000000000001</v>
+      </c>
+      <c r="F176" s="3">
+        <v>0.71560000000000001</v>
+      </c>
+      <c r="G176" s="3">
+        <v>0.70720000000000005</v>
+      </c>
+      <c r="H176" s="3">
+        <v>0.71440000000000003</v>
+      </c>
+      <c r="I176" s="3">
+        <v>0.70520000000000005</v>
+      </c>
+      <c r="J176" s="5">
+        <v>0.72760000000000002</v>
+      </c>
+      <c r="K176" s="3">
+        <v>0.70079999999999998</v>
+      </c>
+      <c r="L176" s="3">
+        <v>0.70240000000000002</v>
+      </c>
+      <c r="N176" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O176" s="2">
+        <v>0.73440000000000005</v>
+      </c>
+      <c r="P176" s="2">
+        <v>0.71079999999999999</v>
+      </c>
+      <c r="Q176" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="R176" s="2">
+        <v>0.73839999999999995</v>
+      </c>
+      <c r="S176" s="2">
+        <v>0.71479999999999999</v>
+      </c>
+      <c r="T176" s="2">
+        <v>0.70920000000000005</v>
+      </c>
+      <c r="U176" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="V176" s="2">
+        <v>0.7268</v>
+      </c>
+      <c r="W176" s="2">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="X176" s="2">
+        <v>0.71679999999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B177" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C177" s="3">
+        <v>0.72160000000000002</v>
+      </c>
+      <c r="D177" s="3">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="E177" s="3">
+        <v>0.71479999999999999</v>
+      </c>
+      <c r="F177" s="3">
+        <v>0.71440000000000003</v>
+      </c>
+      <c r="G177" s="3">
+        <v>0.71160000000000001</v>
+      </c>
+      <c r="H177" s="3">
+        <v>0.70920000000000005</v>
+      </c>
+      <c r="I177" s="3">
+        <v>0.70920000000000005</v>
+      </c>
+      <c r="J177" s="3">
+        <v>0.72319999999999995</v>
+      </c>
+      <c r="K177" s="3">
+        <v>0.70960000000000001</v>
+      </c>
+      <c r="L177" s="3">
+        <v>0.69520000000000004</v>
+      </c>
+      <c r="N177" s="9">
+        <v>1000</v>
+      </c>
+      <c r="O177" s="2">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="P177" s="2">
+        <v>0.71879999999999999</v>
+      </c>
+      <c r="Q177" s="2">
+        <v>0.71360000000000001</v>
+      </c>
+      <c r="R177" s="2">
+        <v>0.73519999999999996</v>
+      </c>
+      <c r="S177" s="2">
+        <v>0.71719999999999995</v>
+      </c>
+      <c r="T177" s="2">
+        <v>0.71279999999999999</v>
+      </c>
+      <c r="U177" s="2">
+        <v>0.70320000000000005</v>
+      </c>
+      <c r="V177" s="2">
+        <v>0.72240000000000004</v>
+      </c>
+      <c r="W177" s="2">
+        <v>0.73319999999999996</v>
+      </c>
+      <c r="X177" s="2">
+        <v>0.72199999999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B178" s="9">
+        <v>2000</v>
+      </c>
+      <c r="C178" s="3">
+        <v>0.71919999999999995</v>
+      </c>
+      <c r="D178" s="3">
+        <v>0.69640000000000002</v>
+      </c>
+      <c r="E178" s="3">
+        <v>0.70679999999999998</v>
+      </c>
+      <c r="F178" s="3">
+        <v>0.71960000000000002</v>
+      </c>
+      <c r="G178" s="3">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="H178" s="3">
+        <v>0.71319999999999995</v>
+      </c>
+      <c r="I178" s="3">
+        <v>0.6956</v>
+      </c>
+      <c r="J178" s="3">
+        <v>0.72440000000000004</v>
+      </c>
+      <c r="K178" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="L178" s="3">
+        <v>0.69640000000000002</v>
+      </c>
+      <c r="N178" s="4">
+        <v>2000</v>
+      </c>
+      <c r="O178" s="5">
+        <v>0.73839999999999995</v>
+      </c>
+      <c r="P178" s="2">
+        <v>0.7248</v>
+      </c>
+      <c r="Q178" s="2">
+        <v>0.71360000000000001</v>
+      </c>
+      <c r="R178" s="2">
+        <v>0.74239999999999995</v>
+      </c>
+      <c r="S178" s="2">
+        <v>0.71479999999999999</v>
+      </c>
+      <c r="T178" s="2">
+        <v>0.70720000000000005</v>
+      </c>
+      <c r="U178" s="2">
+        <v>0.69920000000000004</v>
+      </c>
+      <c r="V178" s="2">
+        <v>0.73280000000000001</v>
+      </c>
+      <c r="W178" s="2">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="X178" s="2">
+        <v>0.70920000000000005</v>
+      </c>
+    </row>
+    <row r="179" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B179" s="9">
+        <v>3000</v>
+      </c>
+      <c r="C179" s="3">
+        <v>0.71719999999999995</v>
+      </c>
+      <c r="D179" s="3">
+        <v>0.69479999999999997</v>
+      </c>
+      <c r="E179" s="3">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="F179" s="3">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="G179" s="3">
+        <v>0.72119999999999995</v>
+      </c>
+      <c r="H179" s="3">
+        <v>0.71719999999999995</v>
+      </c>
+      <c r="I179" s="3">
+        <v>0.70920000000000005</v>
+      </c>
+      <c r="J179" s="3">
+        <v>0.72119999999999995</v>
+      </c>
+      <c r="K179" s="3">
+        <v>0.70079999999999998</v>
+      </c>
+      <c r="L179" s="3">
+        <v>0.6956</v>
+      </c>
+      <c r="N179" s="1">
+        <v>3000</v>
+      </c>
+      <c r="O179" s="2">
+        <v>0.7268</v>
+      </c>
+      <c r="P179" s="2">
+        <v>0.71640000000000004</v>
+      </c>
+      <c r="Q179" s="2">
+        <v>0.71560000000000001</v>
+      </c>
+      <c r="R179" s="3">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="S179" s="2">
+        <v>0.71319999999999995</v>
+      </c>
+      <c r="T179" s="2">
+        <v>0.71120000000000005</v>
+      </c>
+      <c r="U179" s="2">
+        <v>0.69440000000000002</v>
+      </c>
+      <c r="V179" s="2">
+        <v>0.72519999999999996</v>
+      </c>
+      <c r="W179" s="2">
+        <v>0.72840000000000005</v>
+      </c>
+      <c r="X179" s="2">
+        <v>0.73319999999999996</v>
+      </c>
+    </row>
+    <row r="180" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B180" s="8">
+        <v>4000</v>
+      </c>
+      <c r="C180" s="3">
+        <v>0.72040000000000004</v>
+      </c>
+      <c r="D180" s="3">
+        <v>0.69720000000000004</v>
+      </c>
+      <c r="E180" s="3">
+        <v>0.70440000000000003</v>
+      </c>
+      <c r="F180" s="3">
+        <v>0.72760000000000002</v>
+      </c>
+      <c r="G180" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="H180" s="3">
+        <v>0.71279999999999999</v>
+      </c>
+      <c r="I180" s="3">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="J180" s="3">
+        <v>0.71840000000000004</v>
+      </c>
+      <c r="K180" s="3">
+        <v>0.7036</v>
+      </c>
+      <c r="L180" s="3">
+        <v>0.69840000000000002</v>
+      </c>
+      <c r="N180" s="6">
+        <v>4000</v>
+      </c>
+      <c r="O180" s="2">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="P180" s="2">
+        <v>0.71879999999999999</v>
+      </c>
+      <c r="Q180" s="2">
+        <v>0.71040000000000003</v>
+      </c>
+      <c r="R180" s="2">
+        <v>0.73360000000000003</v>
+      </c>
+      <c r="S180" s="2">
+        <v>0.72519999999999996</v>
+      </c>
+      <c r="T180" s="2">
+        <v>0.70679999999999998</v>
+      </c>
+      <c r="U180" s="2">
+        <v>0.68920000000000003</v>
+      </c>
+      <c r="V180" s="2">
+        <v>0.72960000000000003</v>
+      </c>
+      <c r="W180" s="2">
+        <v>0.73519999999999996</v>
+      </c>
+      <c r="X180" s="2">
+        <v>0.72040000000000004</v>
+      </c>
+    </row>
+    <row r="182" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B182" t="s">
+        <v>17</v>
+      </c>
+      <c r="N182" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="183" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B183" t="s">
+        <v>1</v>
+      </c>
+      <c r="N183" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B184" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C184" s="1">
+        <v>0</v>
+      </c>
+      <c r="D184" s="1">
+        <v>1</v>
+      </c>
+      <c r="E184" s="1">
+        <v>2</v>
+      </c>
+      <c r="F184" s="1">
+        <v>3</v>
+      </c>
+      <c r="G184" s="1">
+        <v>4</v>
+      </c>
+      <c r="H184" s="1">
+        <v>5</v>
+      </c>
+      <c r="I184" s="1">
+        <v>6</v>
+      </c>
+      <c r="J184" s="1">
+        <v>7</v>
+      </c>
+      <c r="K184" s="1">
+        <v>8</v>
+      </c>
+      <c r="L184" s="1">
+        <v>9</v>
+      </c>
+      <c r="N184" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O184" s="1">
+        <v>0</v>
+      </c>
+      <c r="P184" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q184" s="1">
+        <v>2</v>
+      </c>
+      <c r="R184" s="1">
+        <v>3</v>
+      </c>
+      <c r="S184" s="1">
+        <v>4</v>
+      </c>
+      <c r="T184" s="1">
+        <v>5</v>
+      </c>
+      <c r="U184" s="1">
+        <v>6</v>
+      </c>
+      <c r="V184" s="1">
+        <v>7</v>
+      </c>
+      <c r="W184" s="1">
+        <v>8</v>
+      </c>
+      <c r="X184" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B185" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C185" s="2">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="D185" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="E185" s="2">
+        <v>0.88624999999999998</v>
+      </c>
+      <c r="F185" s="2">
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="G185" s="2">
+        <v>0.89624999999999999</v>
+      </c>
+      <c r="H185" s="2">
+        <v>0.91874999999999996</v>
+      </c>
+      <c r="I185" s="2">
+        <v>0.90375000000000005</v>
+      </c>
+      <c r="J185" s="2">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="K185" s="2">
+        <v>0.89249999999999996</v>
+      </c>
+      <c r="L185" s="2">
+        <v>0.91749999999999998</v>
+      </c>
+      <c r="N185" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O185" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="P185" s="3">
+        <v>0.86750000000000005</v>
+      </c>
+      <c r="Q185" s="3">
+        <v>0.86375000000000002</v>
+      </c>
+      <c r="R185" s="3">
+        <v>0.86624999999999996</v>
+      </c>
+      <c r="S185" s="3">
+        <v>0.85750000000000004</v>
+      </c>
+      <c r="T185" s="3">
+        <v>0.87375000000000003</v>
+      </c>
+      <c r="U185" s="3">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="V185" s="3">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="W185" s="3">
+        <v>0.85250000000000004</v>
+      </c>
+      <c r="X185" s="3">
+        <v>0.87749999999999995</v>
+      </c>
+    </row>
+    <row r="186" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B186" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C186" s="2">
+        <v>0.90125</v>
+      </c>
+      <c r="D186">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="E186">
+        <v>0.89</v>
+      </c>
+      <c r="F186" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="G186" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="H186" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="I186" s="2">
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="J186" s="5">
+        <v>0.92874999999999996</v>
+      </c>
+      <c r="K186" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="L186" s="3">
+        <v>0.91625000000000001</v>
+      </c>
+      <c r="N186" s="9">
+        <v>1000</v>
+      </c>
+      <c r="O186" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="P186" s="10">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="Q186" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="R186" s="3">
+        <v>0.87624999999999997</v>
+      </c>
+      <c r="S186" s="3">
+        <v>0.85750000000000004</v>
+      </c>
+      <c r="T186" s="3">
+        <v>0.86875000000000002</v>
+      </c>
+      <c r="U186" s="3">
+        <v>0.85624999999999996</v>
+      </c>
+      <c r="V186" s="3">
+        <v>0.87124999999999997</v>
+      </c>
+      <c r="W186" s="3">
+        <v>0.85624999999999996</v>
+      </c>
+      <c r="X186" s="3">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="187" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B187" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C187" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="D187" s="2">
+        <v>0.89624999999999999</v>
+      </c>
+      <c r="E187" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="F187" s="2">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G187" s="2">
+        <v>0.90874999999999995</v>
+      </c>
+      <c r="H187" s="2">
+        <v>0.91125</v>
+      </c>
+      <c r="I187" s="2">
+        <v>0.89124999999999999</v>
+      </c>
+      <c r="J187" s="2">
+        <v>0.92125000000000001</v>
+      </c>
+      <c r="K187" s="2">
+        <v>0.89375000000000004</v>
+      </c>
+      <c r="L187" s="2">
+        <v>0.91625000000000001</v>
+      </c>
+      <c r="N187" s="1">
+        <v>2000</v>
+      </c>
+      <c r="O187" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="P187" s="3">
+        <v>0.87124999999999997</v>
+      </c>
+      <c r="Q187" s="3">
+        <v>0.86750000000000005</v>
+      </c>
+      <c r="R187" s="3">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="S187" s="3">
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="T187" s="3">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="U187" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="V187" s="3">
+        <v>0.86875000000000002</v>
+      </c>
+      <c r="W187" s="3">
+        <v>0.86750000000000005</v>
+      </c>
+      <c r="X187" s="3">
+        <v>0.86750000000000005</v>
+      </c>
+    </row>
+    <row r="188" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B188" s="9">
+        <v>3000</v>
+      </c>
+      <c r="C188" s="2">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="D188" s="2">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="E188" s="2">
+        <v>0.89124999999999999</v>
+      </c>
+      <c r="F188" s="3">
+        <v>0.90375000000000005</v>
+      </c>
+      <c r="G188" s="2">
+        <v>0.89249999999999996</v>
+      </c>
+      <c r="H188" s="2">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="I188" s="2">
+        <v>0.89249999999999996</v>
+      </c>
+      <c r="J188" s="2">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="K188" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="L188" s="2">
+        <v>0.91874999999999996</v>
+      </c>
+      <c r="N188" s="4">
+        <v>3000</v>
+      </c>
+      <c r="O188" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="P188" s="3">
+        <v>0.87375000000000003</v>
+      </c>
+      <c r="Q188" s="3">
+        <v>0.86624999999999996</v>
+      </c>
+      <c r="R188" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="S188" s="3">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="T188" s="3">
+        <v>0.87624999999999997</v>
+      </c>
+      <c r="U188" s="3">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="V188" s="5">
+        <v>0.89</v>
+      </c>
+      <c r="W188" s="3">
+        <v>0.85624999999999996</v>
+      </c>
+      <c r="X188" s="3">
+        <v>0.86624999999999996</v>
+      </c>
+    </row>
+    <row r="189" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B189" s="6">
+        <v>4000</v>
+      </c>
+      <c r="C189" s="2">
+        <v>0.89875000000000005</v>
+      </c>
+      <c r="D189" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="E189" s="2">
+        <v>0.90375000000000005</v>
+      </c>
+      <c r="F189" s="2">
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="G189" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="H189" s="2">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="I189" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="J189" s="2">
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="K189" s="2">
+        <v>0.89749999999999996</v>
+      </c>
+      <c r="L189" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="N189" s="6">
+        <v>4000</v>
+      </c>
+      <c r="O189" s="3">
+        <v>0.87875000000000003</v>
+      </c>
+      <c r="P189" s="3">
+        <v>0.87875000000000003</v>
+      </c>
+      <c r="Q189" s="3">
+        <v>0.85875000000000001</v>
+      </c>
+      <c r="R189" s="3">
+        <v>0.87375000000000003</v>
+      </c>
+      <c r="S189" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="T189" s="3">
+        <v>0.87749999999999995</v>
+      </c>
+      <c r="U189" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="V189" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="W189" s="3">
+        <v>0.84624999999999995</v>
+      </c>
+      <c r="X189" s="3">
+        <v>0.87124999999999997</v>
+      </c>
+    </row>
+    <row r="191" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B191" t="s">
+        <v>2</v>
+      </c>
+      <c r="N191" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B192" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C192" s="1">
+        <v>0</v>
+      </c>
+      <c r="D192" s="1">
+        <v>1</v>
+      </c>
+      <c r="E192" s="1">
+        <v>2</v>
+      </c>
+      <c r="F192" s="1">
+        <v>3</v>
+      </c>
+      <c r="G192" s="1">
+        <v>4</v>
+      </c>
+      <c r="H192" s="1">
+        <v>5</v>
+      </c>
+      <c r="I192" s="1">
+        <v>6</v>
+      </c>
+      <c r="J192" s="1">
+        <v>7</v>
+      </c>
+      <c r="K192" s="1">
+        <v>8</v>
+      </c>
+      <c r="L192" s="1">
+        <v>9</v>
+      </c>
+      <c r="N192" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O192" s="1">
+        <v>0</v>
+      </c>
+      <c r="P192" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q192" s="1">
+        <v>2</v>
+      </c>
+      <c r="R192" s="1">
+        <v>3</v>
+      </c>
+      <c r="S192" s="1">
+        <v>4</v>
+      </c>
+      <c r="T192" s="1">
+        <v>5</v>
+      </c>
+      <c r="U192" s="1">
+        <v>6</v>
+      </c>
+      <c r="V192" s="1">
+        <v>7</v>
+      </c>
+      <c r="W192" s="1">
+        <v>8</v>
+      </c>
+      <c r="X192" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="193" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B193" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C193" s="2">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="D193" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="E193" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="F193" s="2">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="G193" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="H193" s="2">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="I193" s="2">
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="J193" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="K193" s="2">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="L193" s="2">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="N193" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O193" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="P193" s="3">
+        <v>0.66874999999999996</v>
+      </c>
+      <c r="Q193" s="3">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="R193" s="3">
+        <v>0.76875000000000004</v>
+      </c>
+      <c r="S193" s="3">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="T193" s="3">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="U193" s="3">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="V193" s="3">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="W193" s="3">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="X193" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="194" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B194" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C194" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="D194" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E194" s="2">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="F194" s="2">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="G194" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H194" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="I194" s="2">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="J194" s="2">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="K194" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="L194" s="2">
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="N194" s="4">
+        <v>1000</v>
+      </c>
+      <c r="O194" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="P194" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="Q194" s="3">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="R194" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="S194" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="T194" s="3">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="U194" s="3">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="V194" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="W194" s="3">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="X194" s="3">
+        <v>0.73750000000000004</v>
+      </c>
+    </row>
+    <row r="195" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B195" s="4">
+        <v>2000</v>
+      </c>
+      <c r="C195" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="D195" s="2">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E195" s="2">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="F195" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G195" s="5">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="H195" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="I195" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="J195" s="2">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="K195" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="L195" s="2">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="N195" s="1">
+        <v>2000</v>
+      </c>
+      <c r="O195" s="3">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="P195" s="3">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="Q195" s="3">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="R195" s="3">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="S195" s="3">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="T195" s="3">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="U195" s="3">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="V195" s="3">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="W195" s="3">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="X195" s="3">
+        <v>0.76249999999999996</v>
+      </c>
+    </row>
+    <row r="196" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B196" s="9">
+        <v>3000</v>
+      </c>
+      <c r="C196" s="2">
+        <v>0.74375000000000002</v>
+      </c>
+      <c r="D196" s="3">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="E196" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="F196" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G196" s="2">
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="H196" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="I196" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="J196" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="K196" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="L196" s="2">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="N196" s="9">
+        <v>3000</v>
+      </c>
+      <c r="O196" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="P196" s="3">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="Q196" s="3">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="R196" s="3">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="S196" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="T196" s="3">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="U196" s="3">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="V196" s="3">
+        <v>0.70625000000000004</v>
+      </c>
+      <c r="W196" s="3">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="X196" s="3">
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="197" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B197" s="6">
+        <v>4000</v>
+      </c>
+      <c r="C197" s="2">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="D197" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E197" s="2">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="F197" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="G197" s="2">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="H197" s="2">
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="I197" s="2">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="J197" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="K197" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="L197" s="3">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="N197" s="6">
+        <v>4000</v>
+      </c>
+      <c r="O197" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="P197" s="3">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="Q197" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="R197" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="S197" s="3">
+        <v>0.79374999999999996</v>
+      </c>
+      <c r="T197" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="U197" s="3">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="V197" s="3">
+        <v>0.73124999999999996</v>
+      </c>
+      <c r="W197" s="3">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="X197" s="3">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="199" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B199" t="s">
+        <v>3</v>
+      </c>
+      <c r="N199" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B200" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C200" s="1">
+        <v>0</v>
+      </c>
+      <c r="D200" s="1">
+        <v>1</v>
+      </c>
+      <c r="E200" s="1">
+        <v>2</v>
+      </c>
+      <c r="F200" s="1">
+        <v>3</v>
+      </c>
+      <c r="G200" s="1">
+        <v>4</v>
+      </c>
+      <c r="H200" s="1">
+        <v>5</v>
+      </c>
+      <c r="I200" s="1">
+        <v>6</v>
+      </c>
+      <c r="J200" s="1">
+        <v>7</v>
+      </c>
+      <c r="K200" s="1">
+        <v>8</v>
+      </c>
+      <c r="L200" s="1">
+        <v>9</v>
+      </c>
+      <c r="N200" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O200" s="1">
+        <v>0</v>
+      </c>
+      <c r="P200" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q200" s="1">
+        <v>2</v>
+      </c>
+      <c r="R200" s="1">
+        <v>3</v>
+      </c>
+      <c r="S200" s="1">
+        <v>4</v>
+      </c>
+      <c r="T200" s="1">
+        <v>5</v>
+      </c>
+      <c r="U200" s="1">
+        <v>6</v>
+      </c>
+      <c r="V200" s="1">
+        <v>7</v>
+      </c>
+      <c r="W200" s="1">
+        <v>8</v>
+      </c>
+      <c r="X200" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="201" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B201" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C201" s="2">
+        <v>0.79720000000000002</v>
+      </c>
+      <c r="D201" s="2">
+        <v>0.77280000000000004</v>
+      </c>
+      <c r="E201" s="2">
+        <v>0.7772</v>
+      </c>
+      <c r="F201" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="G201" s="2">
+        <v>0.79559999999999997</v>
+      </c>
+      <c r="H201" s="2">
+        <v>0.78720000000000001</v>
+      </c>
+      <c r="I201" s="2">
+        <v>0.78480000000000005</v>
+      </c>
+      <c r="J201" s="2">
+        <v>0.78559999999999997</v>
+      </c>
+      <c r="K201" s="2">
+        <v>0.7772</v>
+      </c>
+      <c r="L201" s="2">
+        <v>0.77880000000000005</v>
+      </c>
+      <c r="N201" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O201" s="5">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="P201" s="3">
+        <v>0.79520000000000002</v>
+      </c>
+      <c r="Q201" s="3">
+        <v>0.78359999999999996</v>
+      </c>
+      <c r="R201" s="3">
+        <v>0.79079999999999995</v>
+      </c>
+      <c r="S201" s="3">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="T201" s="3">
+        <v>0.79079999999999995</v>
+      </c>
+      <c r="U201" s="3">
+        <v>0.78039999999999998</v>
+      </c>
+      <c r="V201" s="3">
+        <v>0.78879999999999995</v>
+      </c>
+      <c r="W201" s="3">
+        <v>0.79879999999999995</v>
+      </c>
+      <c r="X201" s="3">
+        <v>0.78720000000000001</v>
+      </c>
+    </row>
+    <row r="202" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B202" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C202" s="2">
+        <v>0.79279999999999995</v>
+      </c>
+      <c r="D202" s="2">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="E202" s="2">
+        <v>0.7792</v>
+      </c>
+      <c r="F202" s="2">
+        <v>0.78839999999999999</v>
+      </c>
+      <c r="G202" s="2">
+        <v>0.79920000000000002</v>
+      </c>
+      <c r="H202" s="2">
+        <v>0.77359999999999995</v>
+      </c>
+      <c r="I202" s="2">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="J202" s="2">
+        <v>0.78680000000000005</v>
+      </c>
+      <c r="K202" s="2">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="L202" s="2">
+        <v>0.76880000000000004</v>
+      </c>
+      <c r="N202" s="9">
+        <v>1000</v>
+      </c>
+      <c r="O202" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="P202" s="3">
+        <v>0.79920000000000002</v>
+      </c>
+      <c r="Q202" s="3">
+        <v>0.76719999999999999</v>
+      </c>
+      <c r="R202" s="3">
+        <v>0.80079999999999996</v>
+      </c>
+      <c r="S202" s="3">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="T202" s="3">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="U202" s="3">
+        <v>0.78559999999999997</v>
+      </c>
+      <c r="V202" s="3">
+        <v>0.80520000000000003</v>
+      </c>
+      <c r="W202" s="3">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="X202" s="3">
+        <v>0.78959999999999997</v>
+      </c>
+    </row>
+    <row r="203" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="B203" s="4">
+        <v>2000</v>
+      </c>
+      <c r="C203" s="5">
+        <v>0.8024</v>
+      </c>
+      <c r="D203" s="2">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="E203" s="2">
+        <v>0.78120000000000001</v>
+      </c>
+      <c r="F203" s="2">
+        <v>0.78359999999999996</v>
+      </c>
+      <c r="G203" s="2">
+        <v>0.79159999999999997</v>
+      </c>
+      <c r="H203" s="2">
+        <v>0.78559999999999997</v>
+      </c>
+      <c r="I203" s="2">
+        <v>0.77839999999999998</v>
+      </c>
+      <c r="J203" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="K203" s="2">
+        <v>0.79679999999999995</v>
+      </c>
+      <c r="L203" s="2">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="N203" s="9">
+        <v>2000</v>
+      </c>
+      <c r="O203" s="3">
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="P203" s="3">
+        <v>0.79039999999999999</v>
+      </c>
+      <c r="Q203" s="3">
+        <v>0.77439999999999998</v>
+      </c>
+      <c r="R203" s="3">
+        <v>0.79559999999999997</v>
+      </c>
+      <c r="S203" s="3">
+        <v>0.80920000000000003</v>
+      </c>
+      <c r="T203" s="3">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="U203" s="3">
+        <v>0.78239999999999998</v>
+      </c>
+      <c r="V203" s="3">
+        <v>0.80320000000000003</v>
+      </c>
+      <c r="W203" s="3">
+        <v>0.81120000000000003</v>
+      </c>
+      <c r="X203" s="3">
+        <v>0.79520000000000002</v>
+      </c>
+    </row>
+    <row r="204" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B204" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C204" s="2">
+        <v>0.79920000000000002</v>
+      </c>
+      <c r="D204" s="2">
+        <v>0.77039999999999997</v>
+      </c>
+      <c r="E204" s="2">
+        <v>0.78559999999999997</v>
+      </c>
+      <c r="F204" s="3">
+        <v>0.78920000000000001</v>
+      </c>
+      <c r="G204" s="2">
+        <v>0.79959999999999998</v>
+      </c>
+      <c r="H204" s="2">
+        <v>0.78039999999999998</v>
+      </c>
+      <c r="I204" s="2">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="J204" s="2">
+        <v>0.79079999999999995</v>
+      </c>
+      <c r="K204" s="2">
+        <v>0.79679999999999995</v>
+      </c>
+      <c r="L204" s="2">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="N204" s="1">
+        <v>3000</v>
+      </c>
+      <c r="O204" s="3">
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="P204" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="Q204" s="3">
+        <v>0.7772</v>
+      </c>
+      <c r="R204" s="3">
+        <v>0.79920000000000002</v>
+      </c>
+      <c r="S204" s="3">
+        <v>0.80840000000000001</v>
+      </c>
+      <c r="T204" s="3">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="U204" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="V204" s="3">
+        <v>0.79959999999999998</v>
+      </c>
+      <c r="W204" s="3">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="X204" s="3">
+        <v>0.7984</v>
+      </c>
+    </row>
+    <row r="205" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B205" s="6">
+        <v>4000</v>
+      </c>
+      <c r="C205" s="2">
+        <v>0.79279999999999995</v>
+      </c>
+      <c r="D205" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="E205" s="2">
+        <v>0.79359999999999997</v>
+      </c>
+      <c r="F205" s="2">
+        <v>0.79320000000000002</v>
+      </c>
+      <c r="G205" s="2">
+        <v>0.78359999999999996</v>
+      </c>
+      <c r="H205" s="2">
+        <v>0.78359999999999996</v>
+      </c>
+      <c r="I205" s="2">
+        <v>0.77839999999999998</v>
+      </c>
+      <c r="J205" s="2">
+        <v>0.78639999999999999</v>
+      </c>
+      <c r="K205" s="2">
+        <v>0.78559999999999997</v>
+      </c>
+      <c r="L205" s="2">
+        <v>0.78480000000000005</v>
+      </c>
+      <c r="N205" s="6">
+        <v>4000</v>
+      </c>
+      <c r="O205" s="3">
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="P205" s="3">
+        <v>0.78720000000000001</v>
+      </c>
+      <c r="Q205" s="3">
+        <v>0.7772</v>
+      </c>
+      <c r="R205" s="3">
+        <v>0.8024</v>
+      </c>
+      <c r="S205" s="3">
+        <v>0.8044</v>
+      </c>
+      <c r="T205" s="3">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="U205" s="3">
+        <v>0.77880000000000005</v>
+      </c>
+      <c r="V205" s="3">
+        <v>0.79679999999999995</v>
+      </c>
+      <c r="W205" s="3">
+        <v>0.81240000000000001</v>
+      </c>
+      <c r="X205" s="3">
+        <v>0.79600000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>